<commit_message>
Update to Python 3, minor adjustments to shul scheduling
</commit_message>
<xml_diff>
--- a/emptyParshaSheet.xlsx
+++ b/emptyParshaSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private_Files\shul-calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernste\PycharmProjects\shul-calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,9 +464,9 @@
   <tableColumns count="5">
     <tableColumn id="4" name="תאריך" dataDxfId="4"/>
     <tableColumn id="1" name="פרשה" dataDxfId="3"/>
-    <tableColumn id="2" name="בעל קורא" dataDxfId="2"/>
-    <tableColumn id="3" name="תורם סעודה שלישית" dataDxfId="1"/>
-    <tableColumn id="5" name="דבר תורה ליל שבת" dataDxfId="0"/>
+    <tableColumn id="2" name="דבר תורה ליל שבת" dataDxfId="2"/>
+    <tableColumn id="3" name="בעל קורא" dataDxfId="1"/>
+    <tableColumn id="5" name="תורם סעודה שלישית" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -762,7 +762,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,20 +781,20 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4"/>
       <c r="E2" s="8"/>
     </row>

</xml_diff>